<commit_message>
Commenced series data analysis
</commit_message>
<xml_diff>
--- a/input/raw_data/final_report/bib_search_screen_end.xlsx
+++ b/input/raw_data/final_report/bib_search_screen_end.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackgedge/Projects/msc_dissertation/iifo_motivation/input/raw_data/final_report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF27FE91-7CAC-2640-B819-FE17F1DE9C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E0342C-DA6D-5540-A5FC-842D13FFF75C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20520" yWindow="880" windowWidth="20600" windowHeight="24440" xr2:uid="{2024F0F2-C7A4-0040-8726-2BCD36CB7E46}"/>
   </bookViews>
@@ -4056,9 +4056,9 @@
   <dimension ref="A1:U195"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="N1" sqref="N1"/>
-      <selection pane="bottomLeft" activeCell="D91" sqref="D91"/>
+      <selection pane="bottomLeft" activeCell="D152" sqref="D152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>